<commit_message>
updated analysis with new points
</commit_message>
<xml_diff>
--- a/Data/Features_Overview.xlsx
+++ b/Data/Features_Overview.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robin\work\conferences\2020_ESSE\comparison\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saile\OneDrive - Otto-Friedrich-Universität Bamberg\ms-framework-comparison\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00DD3B4B-7414-44A5-92CD-1B68D0A12467}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99375C89-6F4C-4DF9-922C-0ED7B1AD5D5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="54">
   <si>
     <t>JAVA</t>
   </si>
@@ -167,32 +167,41 @@
     <t>2.1 CQRS</t>
   </si>
   <si>
-    <t>3.1 Interface specification</t>
-  </si>
-  <si>
     <t>4. Smart Endpoints and Dumb Pipes</t>
   </si>
   <si>
     <t>4.1 API Gateway</t>
   </si>
   <si>
-    <t>4.4 Service coordination</t>
-  </si>
-  <si>
     <t>7.2 Testing</t>
   </si>
   <si>
-    <t>7.3 Continous Deployment</t>
-  </si>
-  <si>
     <t>8.1 Versioning</t>
+  </si>
+  <si>
+    <t>3.1 Interface Specification</t>
+  </si>
+  <si>
+    <t>4.4 Service Coordination</t>
+  </si>
+  <si>
+    <t>7.3 Continuous Deployment</t>
+  </si>
+  <si>
+    <t>NODE.JS</t>
+  </si>
+  <si>
+    <t>Devis</t>
+  </si>
+  <si>
+    <t>Moleculer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -243,8 +252,19 @@
       <color theme="7"/>
       <name val="CMU Serif"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="CMU Serif"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -281,8 +301,26 @@
         <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor rgb="FFBFBFBF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -342,11 +380,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -378,37 +444,19 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -418,6 +466,50 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -800,47 +892,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L35"/>
+  <dimension ref="A1:N35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q12" sqref="Q12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O19" sqref="O19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.5703125" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" customWidth="1"/>
-    <col min="4" max="5" width="10.5703125" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" customWidth="1"/>
+    <col min="1" max="1" width="28.5546875" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" customWidth="1"/>
+    <col min="4" max="5" width="10.5546875" customWidth="1"/>
+    <col min="6" max="6" width="13.88671875" customWidth="1"/>
     <col min="7" max="7" width="16" customWidth="1"/>
-    <col min="8" max="8" width="8.7109375" customWidth="1"/>
-    <col min="9" max="1022" width="10.5703125" customWidth="1"/>
+    <col min="8" max="8" width="8.6640625" customWidth="1"/>
+    <col min="9" max="13" width="10.5546875" customWidth="1"/>
+    <col min="14" max="14" width="14.5546875" customWidth="1"/>
+    <col min="15" max="1022" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="17.45" customHeight="1">
+    <row r="1" spans="1:14" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="2"/>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="12" t="s">
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12" t="s">
+      <c r="I1" s="15"/>
+      <c r="J1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="12"/>
+      <c r="K1" s="15"/>
       <c r="L1" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:12">
+      <c r="M1" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="N1" s="31"/>
+    </row>
+    <row r="2" spans="1:14" ht="15.6" x14ac:dyDescent="0.4">
       <c r="A2" s="4" t="s">
         <v>37</v>
       </c>
@@ -875,8 +973,14 @@
         <v>13</v>
       </c>
       <c r="L2" s="5"/>
-    </row>
-    <row r="3" spans="1:12" ht="30">
+      <c r="M2" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="15.6" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>17</v>
       </c>
@@ -891,8 +995,10 @@
       <c r="J3" s="6"/>
       <c r="K3" s="6"/>
       <c r="L3" s="1"/>
-    </row>
-    <row r="4" spans="1:12" ht="29.25">
+      <c r="M3" s="33"/>
+      <c r="N3" s="33"/>
+    </row>
+    <row r="4" spans="1:14" ht="15.6" x14ac:dyDescent="0.4">
       <c r="A4" s="7" t="s">
         <v>18</v>
       </c>
@@ -929,8 +1035,10 @@
       <c r="L4" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:12">
+      <c r="M4" s="33"/>
+      <c r="N4" s="33"/>
+    </row>
+    <row r="5" spans="1:14" ht="15.6" x14ac:dyDescent="0.4">
       <c r="A5" s="7" t="s">
         <v>20</v>
       </c>
@@ -967,9 +1075,11 @@
       <c r="L5" s="10" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:12">
-      <c r="A6" s="18" t="s">
+      <c r="M5" s="33"/>
+      <c r="N5" s="33"/>
+    </row>
+    <row r="6" spans="1:14" ht="15.6" x14ac:dyDescent="0.4">
+      <c r="A6" s="13" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="9" t="s">
@@ -1003,8 +1113,10 @@
       <c r="L6" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:12">
+      <c r="M6" s="33"/>
+      <c r="N6" s="33"/>
+    </row>
+    <row r="7" spans="1:14" ht="15.6" x14ac:dyDescent="0.4">
       <c r="A7" s="7" t="s">
         <v>42</v>
       </c>
@@ -1041,112 +1153,128 @@
       <c r="L7" s="10" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="1:12">
+      <c r="M7" s="33"/>
+      <c r="N7" s="33"/>
+    </row>
+    <row r="8" spans="1:14" ht="15.6" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="14"/>
-      <c r="C8" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="H8" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I8" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="J8" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="K8" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="L8" s="13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
+      <c r="B8" s="19"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="33"/>
+      <c r="N8" s="33"/>
+    </row>
+    <row r="9" spans="1:14" ht="15.6" x14ac:dyDescent="0.4">
       <c r="A9" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B9" s="14"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
-    </row>
-    <row r="10" spans="1:12">
+      <c r="B9" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="I9" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="J9" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="K9" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="L9" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="M9" s="33"/>
+      <c r="N9" s="33"/>
+    </row>
+    <row r="10" spans="1:14" ht="15.6" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="19"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="19"/>
-      <c r="J10" s="19"/>
-      <c r="K10" s="19"/>
-      <c r="L10" s="19"/>
-    </row>
-    <row r="11" spans="1:12">
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="33"/>
+      <c r="N10" s="33"/>
+    </row>
+    <row r="11" spans="1:14" ht="15.6" x14ac:dyDescent="0.4">
       <c r="A11" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="I11" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="J11" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="K11" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="L11" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="M11" s="33"/>
+      <c r="N11" s="33"/>
+    </row>
+    <row r="12" spans="1:14" ht="31.2" x14ac:dyDescent="0.4">
+      <c r="A12" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="B11" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="F11" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="G11" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="H11" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="I11" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="J11" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="K11" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="L11" s="15" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="30">
-      <c r="A12" s="2" t="s">
-        <v>45</v>
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -1159,46 +1287,50 @@
       <c r="J12" s="6"/>
       <c r="K12" s="6"/>
       <c r="L12" s="1"/>
-    </row>
-    <row r="13" spans="1:12">
+      <c r="M12" s="33"/>
+      <c r="N12" s="33"/>
+    </row>
+    <row r="13" spans="1:14" ht="15.6" x14ac:dyDescent="0.4">
       <c r="A13" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="B13" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="E13" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="F13" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="G13" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="H13" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="I13" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="J13" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="K13" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="L13" s="15" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12">
+        <v>45</v>
+      </c>
+      <c r="B13" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="H13" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="I13" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="J13" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="K13" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="L13" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="M13" s="33"/>
+      <c r="N13" s="33"/>
+    </row>
+    <row r="14" spans="1:14" ht="15.6" x14ac:dyDescent="0.4">
       <c r="A14" s="7" t="s">
         <v>21</v>
       </c>
@@ -1235,8 +1367,10 @@
       <c r="L14" s="9" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="15" spans="1:12">
+      <c r="M14" s="33"/>
+      <c r="N14" s="33"/>
+    </row>
+    <row r="15" spans="1:14" ht="15.6" x14ac:dyDescent="0.4">
       <c r="A15" s="7" t="s">
         <v>22</v>
       </c>
@@ -1273,24 +1407,28 @@
       <c r="L15" s="9" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="16" spans="1:12">
+      <c r="M15" s="33"/>
+      <c r="N15" s="33"/>
+    </row>
+    <row r="16" spans="1:14" ht="15.6" x14ac:dyDescent="0.4">
       <c r="A16" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="B16" s="15"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="16"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="15"/>
-      <c r="K16" s="15"/>
-      <c r="L16" s="15"/>
-    </row>
-    <row r="17" spans="1:12" ht="30">
+        <v>49</v>
+      </c>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="32"/>
+      <c r="N16" s="32"/>
+    </row>
+    <row r="17" spans="1:14" ht="31.2" x14ac:dyDescent="0.4">
       <c r="A17" s="2" t="s">
         <v>33</v>
       </c>
@@ -1305,16 +1443,18 @@
       <c r="J17" s="6"/>
       <c r="K17" s="6"/>
       <c r="L17" s="1"/>
-    </row>
-    <row r="18" spans="1:12">
+      <c r="M17" s="33"/>
+      <c r="N17" s="33"/>
+    </row>
+    <row r="18" spans="1:14" ht="15.6" x14ac:dyDescent="0.4">
       <c r="A18" s="7" t="s">
         <v>23</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="9" t="s">
-        <v>15</v>
+      <c r="C18" s="10" t="s">
+        <v>16</v>
       </c>
       <c r="D18" s="9" t="s">
         <v>15</v>
@@ -1334,17 +1474,19 @@
       <c r="I18" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="J18" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="K18" s="8" t="s">
-        <v>14</v>
+      <c r="J18" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K18" s="10" t="s">
+        <v>16</v>
       </c>
       <c r="L18" s="9" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="19" spans="1:12">
+      <c r="M18" s="33"/>
+      <c r="N18" s="33"/>
+    </row>
+    <row r="19" spans="1:14" ht="15.6" x14ac:dyDescent="0.4">
       <c r="A19" s="2" t="s">
         <v>34</v>
       </c>
@@ -1359,8 +1501,10 @@
       <c r="J19" s="6"/>
       <c r="K19" s="6"/>
       <c r="L19" s="1"/>
-    </row>
-    <row r="20" spans="1:12">
+      <c r="M19" s="33"/>
+      <c r="N19" s="33"/>
+    </row>
+    <row r="20" spans="1:14" ht="15.6" x14ac:dyDescent="0.4">
       <c r="A20" s="7" t="s">
         <v>24</v>
       </c>
@@ -1397,8 +1541,10 @@
       <c r="L20" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="21" spans="1:12">
+      <c r="M20" s="33"/>
+      <c r="N20" s="33"/>
+    </row>
+    <row r="21" spans="1:14" ht="15.6" x14ac:dyDescent="0.4">
       <c r="A21" s="7" t="s">
         <v>25</v>
       </c>
@@ -1435,8 +1581,10 @@
       <c r="L21" s="9" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="22" spans="1:12">
+      <c r="M21" s="33"/>
+      <c r="N21" s="33"/>
+    </row>
+    <row r="22" spans="1:14" ht="15.6" x14ac:dyDescent="0.4">
       <c r="A22" s="7" t="s">
         <v>26</v>
       </c>
@@ -1473,8 +1621,10 @@
       <c r="L22" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="23" spans="1:12">
+      <c r="M22" s="33"/>
+      <c r="N22" s="33"/>
+    </row>
+    <row r="23" spans="1:14" ht="15.6" x14ac:dyDescent="0.4">
       <c r="A23" s="7" t="s">
         <v>27</v>
       </c>
@@ -1511,8 +1661,10 @@
       <c r="L23" s="9" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="24" spans="1:12">
+      <c r="M23" s="33"/>
+      <c r="N23" s="33"/>
+    </row>
+    <row r="24" spans="1:14" ht="15.6" x14ac:dyDescent="0.4">
       <c r="A24" s="7" t="s">
         <v>28</v>
       </c>
@@ -1549,8 +1701,10 @@
       <c r="L24" s="9" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="25" spans="1:12">
+      <c r="M24" s="33"/>
+      <c r="N24" s="33"/>
+    </row>
+    <row r="25" spans="1:14" ht="15.6" x14ac:dyDescent="0.4">
       <c r="A25" s="7" t="s">
         <v>41</v>
       </c>
@@ -1587,8 +1741,10 @@
       <c r="L25" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="26" spans="1:12">
+      <c r="M25" s="33"/>
+      <c r="N25" s="33"/>
+    </row>
+    <row r="26" spans="1:14" ht="15.6" x14ac:dyDescent="0.4">
       <c r="A26" s="7" t="s">
         <v>29</v>
       </c>
@@ -1625,42 +1781,36 @@
       <c r="L26" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="27" spans="1:12">
+      <c r="M26" s="33"/>
+      <c r="N26" s="33"/>
+    </row>
+    <row r="27" spans="1:14" ht="15.6" x14ac:dyDescent="0.4">
       <c r="A27" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B27" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D27" s="8" t="s">
-        <v>14</v>
-      </c>
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
       <c r="G27" s="6"/>
-      <c r="H27" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="I27" s="8" t="s">
-        <v>14</v>
-      </c>
+      <c r="H27" s="8"/>
+      <c r="I27" s="8"/>
       <c r="J27" s="6"/>
       <c r="K27" s="6"/>
       <c r="L27" s="1"/>
-    </row>
-    <row r="28" spans="1:12">
+      <c r="M27" s="33"/>
+      <c r="N27" s="33"/>
+    </row>
+    <row r="28" spans="1:14" ht="15.6" x14ac:dyDescent="0.4">
       <c r="A28" s="7" t="s">
         <v>30</v>
       </c>
       <c r="B28" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C28" s="8" t="s">
-        <v>14</v>
+      <c r="C28" s="9" t="s">
+        <v>15</v>
       </c>
       <c r="D28" s="8" t="s">
         <v>14</v>
@@ -1689,245 +1839,324 @@
       <c r="L28" s="9" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="29" spans="1:12">
+      <c r="M28" s="33"/>
+      <c r="N28" s="33"/>
+    </row>
+    <row r="29" spans="1:14" ht="15.6" x14ac:dyDescent="0.4">
       <c r="A29" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="B29" s="13"/>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="15"/>
-      <c r="F29" s="15"/>
-      <c r="G29" s="15"/>
-      <c r="H29" s="13"/>
-      <c r="I29" s="13"/>
-      <c r="J29" s="15"/>
-      <c r="K29" s="15"/>
-      <c r="L29" s="15"/>
-    </row>
-    <row r="30" spans="1:12">
+        <v>46</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E29" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F29" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G29" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H29" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I29" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J29" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K29" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="L29" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="M29" s="33"/>
+      <c r="N29" s="33"/>
+    </row>
+    <row r="30" spans="1:14" ht="15.6" x14ac:dyDescent="0.4">
       <c r="A30" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="B30" s="13"/>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="15"/>
-      <c r="F30" s="15"/>
-      <c r="G30" s="15"/>
-      <c r="H30" s="13"/>
-      <c r="I30" s="13"/>
-      <c r="J30" s="15"/>
-      <c r="K30" s="15"/>
-      <c r="L30" s="15"/>
-    </row>
-    <row r="31" spans="1:12">
+        <v>50</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F30" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G30" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H30" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I30" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="J30" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K30" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="L30" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="M30" s="33"/>
+      <c r="N30" s="33"/>
+    </row>
+    <row r="31" spans="1:14" ht="15.6" x14ac:dyDescent="0.4">
       <c r="A31" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B31" s="19"/>
-      <c r="C31" s="19"/>
-      <c r="D31" s="19"/>
-      <c r="E31" s="19"/>
-      <c r="F31" s="19"/>
-      <c r="G31" s="19"/>
-      <c r="H31" s="19"/>
-      <c r="I31" s="19"/>
-      <c r="J31" s="19"/>
-      <c r="K31" s="19"/>
-      <c r="L31" s="19"/>
-    </row>
-    <row r="32" spans="1:12">
-      <c r="A32" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="B32" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C32" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="D32" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="E32" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="F32" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="G32" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="H32" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I32" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="J32" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="K32" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="L32" s="13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12">
-      <c r="A33" s="20" t="s">
+      <c r="B31" s="14"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="14"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="14"/>
+      <c r="I31" s="14"/>
+      <c r="J31" s="14"/>
+      <c r="K31" s="14"/>
+      <c r="L31" s="14"/>
+      <c r="M31" s="33"/>
+      <c r="N31" s="33"/>
+    </row>
+    <row r="32" spans="1:14" ht="16.2" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A32" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="B32" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C32" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="D32" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="E32" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="F32" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="G32" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="H32" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="I32" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="J32" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="K32" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="L32" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="M32" s="34"/>
+      <c r="N32" s="34"/>
+    </row>
+    <row r="33" spans="1:14" ht="16.2" thickTop="1" x14ac:dyDescent="0.4">
+      <c r="A33" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="B33" s="17">
+      <c r="B33" s="23">
         <f>COUNTIF(B4:B32,"✓")</f>
+        <v>14</v>
+      </c>
+      <c r="C33" s="23">
+        <f t="shared" ref="B33:L33" si="0">COUNTIF(C4:C32,"✓")</f>
+        <v>5</v>
+      </c>
+      <c r="D33" s="23">
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="C33" s="17">
-        <f>COUNTIF(C4:C32,"✓")</f>
-        <v>5</v>
-      </c>
-      <c r="D33" s="17">
-        <f>COUNTIF(D4:D32,"✓")</f>
-        <v>12</v>
-      </c>
-      <c r="E33" s="17">
-        <f>COUNTIF(E4:E32,"✓")</f>
-        <v>15</v>
-      </c>
-      <c r="F33" s="17">
-        <f>COUNTIF(F4:F32,"✓")</f>
+      <c r="E33" s="23">
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="G33" s="17">
-        <f>COUNTIF(G4:G32,"✓")</f>
-        <v>17</v>
-      </c>
-      <c r="H33" s="17">
-        <f>COUNTIF(H4:H32,"✓")</f>
-        <v>6</v>
-      </c>
-      <c r="I33" s="17">
-        <f>COUNTIF(I4:I32,"✓")</f>
+      <c r="F33" s="23">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="G33" s="23">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="H33" s="23">
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="J33" s="17">
-        <f>COUNTIF(J4:J32,"✓")</f>
+      <c r="I33" s="23">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="J33" s="23">
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="K33" s="17">
-        <f>COUNTIF(K4:K32,"✓")</f>
-        <v>12</v>
-      </c>
-      <c r="L33" s="17">
-        <f>COUNTIF(L4:L32,"✓")</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12">
-      <c r="A34" s="11" t="s">
+      <c r="K33" s="23">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="L33" s="23">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="M33" s="23">
+        <f t="shared" ref="M33" si="1">COUNTIF(M4:M32,"✓")</f>
+        <v>0</v>
+      </c>
+      <c r="N33" s="23">
+        <f t="shared" ref="N33" si="2">COUNTIF(N4:N32,"✓")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" ht="15.6" x14ac:dyDescent="0.4">
+      <c r="A34" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="B34" s="17">
-        <f>COUNTIF(B4:B32,"–")</f>
+      <c r="B34" s="22">
+        <f t="shared" ref="B34:N34" si="3">COUNTIF(B4:B32,"–")</f>
         <v>4</v>
       </c>
-      <c r="C34" s="17">
-        <f>COUNTIF(C4:C32,"–")</f>
-        <v>14</v>
-      </c>
-      <c r="D34" s="17">
+      <c r="C34" s="22">
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
+      <c r="D34" s="22">
         <f>COUNTIF(D4:D32,"–")</f>
         <v>7</v>
       </c>
-      <c r="E34" s="17">
-        <f>COUNTIF(E4:E32,"–")</f>
+      <c r="E34" s="22">
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="F34" s="17">
-        <f>COUNTIF(F4:F32,"–")</f>
+      <c r="F34" s="22">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="G34" s="22">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="H34" s="22">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="I34" s="22">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="J34" s="22">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="K34" s="22">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="L34" s="22">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="M34" s="22">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G34" s="17">
-        <f>COUNTIF(G4:G32,"–")</f>
+      <c r="N34" s="22">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" ht="15.6" x14ac:dyDescent="0.4">
+      <c r="A35" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="B35" s="22">
+        <f t="shared" ref="B35:N35" si="4">COUNTIF(B4:B32,"✗")</f>
+        <v>3</v>
+      </c>
+      <c r="C35" s="22">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="D35" s="22">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="E35" s="22">
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="H34" s="17">
-        <f>COUNTIF(H4:H32,"–")</f>
-        <v>6</v>
-      </c>
-      <c r="I34" s="17">
-        <f>COUNTIF(I4:I32,"–")</f>
-        <v>10</v>
-      </c>
-      <c r="J34" s="17">
-        <f>COUNTIF(J4:J32,"–")</f>
-        <v>7</v>
-      </c>
-      <c r="K34" s="17">
-        <f>COUNTIF(K4:K32,"–")</f>
-        <v>6</v>
-      </c>
-      <c r="L34" s="17">
-        <f>COUNTIF(L4:L32,"–")</f>
+      <c r="F35" s="22">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G35" s="22">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H35" s="22">
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="35" spans="1:12">
-      <c r="A35" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="B35" s="17">
-        <f>COUNTIF(B4:B32,"✗")</f>
+      <c r="I35" s="22">
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
-      <c r="C35" s="17">
-        <f>COUNTIF(C4:C32,"✗")</f>
-        <v>1</v>
-      </c>
-      <c r="D35" s="17">
-        <f>COUNTIF(D4:D32,"✗")</f>
-        <v>1</v>
-      </c>
-      <c r="E35" s="17">
-        <f>COUNTIF(E4:E32,"✗")</f>
-        <v>1</v>
-      </c>
-      <c r="F35" s="17">
-        <f>COUNTIF(F4:F32,"✗")</f>
+      <c r="J35" s="22">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="K35" s="22">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="L35" s="22">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="M35" s="22">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="G35" s="17">
-        <f>COUNTIF(G4:G32,"✗")</f>
+      <c r="N35" s="22">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="H35" s="17">
-        <f>COUNTIF(H4:H32,"✗")</f>
-        <v>8</v>
-      </c>
-      <c r="I35" s="17">
-        <f>COUNTIF(I4:I32,"✗")</f>
-        <v>3</v>
-      </c>
-      <c r="J35" s="17">
-        <f>COUNTIF(J4:J32,"✗")</f>
-        <v>1</v>
-      </c>
-      <c r="K35" s="17">
-        <f>COUNTIF(K4:K32,"✗")</f>
-        <v>1</v>
-      </c>
-      <c r="L35" s="17">
-        <f>COUNTIF(L4:L32,"✗")</f>
-        <v>2</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="B1:G1"/>
+    <mergeCell ref="M1:N1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>